<commit_message>
Mapping Profit Centers Locally
</commit_message>
<xml_diff>
--- a/app/data/Profit Center Mapping.xlsx
+++ b/app/data/Profit Center Mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raul.Sharma\Documents\GitHub\gpi-demo\app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://graphicpkg-my.sharepoint.com/personal/raul_sharma_graphicpkg_com/Documents/Documents/GitHub/gpi-demo/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{F08D388A-C29E-4D1B-8E63-B716C8294F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="340" windowWidth="17050" windowHeight="7190" tabRatio="798" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="798" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cognos_Office_Connection_Cache" sheetId="8" state="veryHidden" r:id="rId1"/>
@@ -1747,9 +1747,9 @@
   </sheetPr>
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added Functionality and Renamed Files
</commit_message>
<xml_diff>
--- a/app/data/Profit Center Mapping.xlsx
+++ b/app/data/Profit Center Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://graphicpkg-my.sharepoint.com/personal/raul_sharma_graphicpkg_com/Documents/Documents/GitHub/gpi-demo/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F08D388A-C29E-4D1B-8E63-B716C8294F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{F08D388A-C29E-4D1B-8E63-B716C8294F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{550674DC-F6CE-48A3-98EA-97DA28E44923}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="798" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6990" yWindow="2450" windowWidth="14400" windowHeight="7360" tabRatio="798" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cognos_Office_Connection_Cache" sheetId="8" state="veryHidden" r:id="rId1"/>
@@ -1748,8 +1748,8 @@
   <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G86"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -1786,113 +1786,113 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>316</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="11">
+        <v>32169</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
+      <c r="A3" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>219</v>
+        <v>290</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>1</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>218</v>
+        <v>299</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>221</v>
+        <v>143</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>43</v>
+      <c r="A5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>5</v>
+        <v>259</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>303</v>
@@ -1903,134 +1903,134 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>225</v>
+        <v>264</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>162</v>
+        <v>59</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>162</v>
+        <v>59</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>163</v>
+        <v>58</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
+      <c r="A8" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>303</v>
@@ -2041,42 +2041,42 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>186</v>
+        <v>26</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>186</v>
+        <v>26</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>187</v>
+        <v>25</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>303</v>
@@ -2087,114 +2087,114 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>138</v>
+        <v>44</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>138</v>
+        <v>44</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>303</v>
-      </c>
       <c r="G18" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>310</v>
@@ -2202,19 +2202,19 @@
     </row>
     <row r="20" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>303</v>
@@ -2225,19 +2225,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>307</v>
@@ -2246,21 +2246,21 @@
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>303</v>
@@ -2269,320 +2269,320 @@
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>27</v>
+        <v>217</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>241</v>
+        <v>275</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>188</v>
+        <v>71</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>188</v>
+        <v>71</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>189</v>
+        <v>70</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>242</v>
+        <v>276</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>32</v>
+        <v>152</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>32</v>
+        <v>152</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>31</v>
+        <v>153</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>217</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>146</v>
+        <v>41</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>146</v>
+        <v>41</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>147</v>
+        <v>40</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>307</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>303</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="11">
-        <v>32169</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>247</v>
+      <c r="A30" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>303</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>307</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>158</v>
+        <v>68</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>158</v>
+        <v>68</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>159</v>
+        <v>67</v>
       </c>
       <c r="F33" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="G33" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>303</v>
-      </c>
       <c r="G34" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>300</v>
+        <v>66</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>114</v>
+        <v>226</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>307</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>303</v>
@@ -2593,19 +2593,19 @@
     </row>
     <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>192</v>
+        <v>156</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>192</v>
+        <v>156</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>307</v>
@@ -2616,19 +2616,19 @@
     </row>
     <row r="38" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>307</v>
@@ -2637,47 +2637,47 @@
         <v>310</v>
       </c>
     </row>
-    <row r="39" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="9" t="s">
-        <v>301</v>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>183</v>
+        <v>263</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>211</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>307</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="40" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>202</v>
+        <v>23</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>202</v>
+        <v>23</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>310</v>
@@ -2685,19 +2685,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>307</v>
@@ -2706,67 +2706,67 @@
         <v>310</v>
       </c>
     </row>
-    <row r="42" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>50</v>
+        <v>288</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>49</v>
+        <v>205</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>303</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>53</v>
+        <v>269</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>53</v>
+        <v>168</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>52</v>
+        <v>169</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>303</v>
@@ -2775,21 +2775,21 @@
         <v>310</v>
       </c>
     </row>
-    <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>307</v>
@@ -2798,205 +2798,205 @@
         <v>310</v>
       </c>
     </row>
-    <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>307</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>54</v>
+        <v>300</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>211</v>
+        <v>114</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>307</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>303</v>
+      </c>
+      <c r="G48" s="23" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
-        <v>60</v>
+        <v>215</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>61</v>
+        <v>267</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>115</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>170</v>
+        <v>35</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>170</v>
+        <v>35</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>171</v>
+        <v>34</v>
       </c>
       <c r="F50" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="G50" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E51" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="F51" s="23" t="s">
-        <v>303</v>
-      </c>
-      <c r="G51" s="23" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G51" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
-        <v>215</v>
+        <v>12</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>115</v>
+        <v>229</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="F52" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="G52" s="8" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="E53" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>308</v>
-      </c>
-      <c r="G53" s="16" t="s">
-        <v>311</v>
+      <c r="G53" s="8" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>303</v>
@@ -3005,21 +3005,21 @@
         <v>310</v>
       </c>
     </row>
-    <row r="55" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>307</v>
@@ -3028,24 +3028,24 @@
         <v>310</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>165</v>
+        <v>46</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>310</v>
@@ -3053,111 +3053,111 @@
     </row>
     <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>71</v>
+        <v>192</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>71</v>
+        <v>192</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="59" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>283</v>
+    <row r="59" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>284</v>
+        <v>45</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>77</v>
+        <v>202</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>77</v>
+        <v>202</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>76</v>
+        <v>203</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="61" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>307</v>
@@ -3167,342 +3167,342 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>310</v>
+      <c r="A62" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="63" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B64" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C64" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D64" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E64" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F63" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="G63" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="F64" s="5" t="s">
         <v>303</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>200</v>
+        <v>92</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>200</v>
+        <v>92</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>201</v>
+        <v>91</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>286</v>
+        <v>104</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>291</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>303</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>148</v>
+        <v>292</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>289</v>
+        <v>106</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>293</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>303</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>310</v>
+      <c r="A70" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E70" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="71" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>303</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>94</v>
+        <v>297</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>205</v>
+        <v>129</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>303</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>169</v>
+        <v>112</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="G74" s="16" t="s">
-        <v>304</v>
+        <v>314</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="G75" s="16" t="s">
-        <v>304</v>
+      <c r="A75" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="76" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>290</v>
+        <v>87</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>289</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>303</v>
@@ -3511,211 +3511,211 @@
         <v>310</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="F77" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F78" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="G77" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>303</v>
-      </c>
       <c r="G78" s="8" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>118</v>
+        <v>75</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>303</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
-        <v>107</v>
+        <v>216</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>122</v>
+        <v>198</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>122</v>
+        <v>198</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>123</v>
+        <v>199</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="B82" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="C82" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="D82" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="E82" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="F82" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="G82" s="20" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="G82" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="6" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>126</v>
+        <v>200</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>126</v>
+        <v>200</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="84" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>313</v>
+      <c r="A84" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="G84" s="16" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="85" spans="1:7" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="G85" s="8" t="s">
-        <v>314</v>
+      <c r="A85" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="G85" s="16" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -3742,7 +3742,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G86" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:G86" xr:uid="{00000000-0009-0000-0000-000004000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G86">
+      <sortCondition ref="B1:B86"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="54" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added functionality to change mapping from errors window
</commit_message>
<xml_diff>
--- a/app/data/Profit Center Mapping.xlsx
+++ b/app/data/Profit Center Mapping.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{F08D388A-C29E-4D1B-8E63-B716C8294F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{550674DC-F6CE-48A3-98EA-97DA28E44923}"/>
   <bookViews>
-    <workbookView xWindow="6990" yWindow="2450" windowWidth="14400" windowHeight="7360" tabRatio="798" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="850" windowWidth="14400" windowHeight="7360" tabRatio="798" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cognos_Office_Connection_Cache" sheetId="8" state="veryHidden" r:id="rId1"/>
@@ -1747,9 +1747,9 @@
   </sheetPr>
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>

</xml_diff>